<commit_message>
New table row column
</commit_message>
<xml_diff>
--- a/src/test/resources/test1.xlsx
+++ b/src/test/resources/test1.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nrjryka\IdeaProjects\exceler\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local_data\app\msys64\home\nrjryka\Home\IdeaProjects\exceler\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="6075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="6075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="shapes" sheetId="3" r:id="rId1"/>
     <sheet name="table" sheetId="4" r:id="rId2"/>
     <sheet name="stack" sheetId="5" r:id="rId3"/>
+    <sheet name="border" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>key</t>
   </si>
@@ -98,6 +99,10 @@
   </si>
   <si>
     <t>val13-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
@@ -322,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -352,6 +357,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2680,7 +2688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2973,4 +2981,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="28"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="28"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="28"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="28"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>